<commit_message>
Adding Notations to Lab 23, it can't be completed
</commit_message>
<xml_diff>
--- a/23_asphyxia/23_asphyxia_data.xlsx
+++ b/23_asphyxia/23_asphyxia_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Asphyxia Test</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>7.41/7.41</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>120/79</t>
+  </si>
+  <si>
+    <t>The workaround available that allowed this lab to be completed in QCP is not present in HumMod.</t>
   </si>
 </sst>
 </file>
@@ -97,12 +109,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -193,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -218,6 +236,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,20 +537,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -542,8 +578,23 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="60.75" thickBot="1">
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -559,8 +610,17 @@
       <c r="E3" s="5">
         <v>40795</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="75.75" thickBot="1">
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="75.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -576,8 +636,17 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5468</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -593,8 +662,17 @@
       <c r="E5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="4">
+        <v>72</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="45.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -610,8 +688,17 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45.75" thickBot="1">
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="4">
+        <v>76</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="45.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -627,8 +714,17 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4">
+        <v>93</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="45">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
@@ -644,8 +740,17 @@
       <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="30.75" thickBot="1">
+      <c r="H8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" ht="30.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -653,13 +758,40 @@
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
+      <c r="H9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="A11:K11"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>